<commit_message>
Constants , Messages , Extended Report Added
</commit_message>
<xml_diff>
--- a/ProjectFinal/src/main/resources/Test_Data.xlsx
+++ b/ProjectFinal/src/main/resources/Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>We have e-mailed your password reset link!</t>
   </si>
   <si>
-    <t xml:space="preserve"> Specialist</t>
+    <t xml:space="preserve"> jamesthomas@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,6 +472,9 @@
       </c>
       <c r="C1" t="s">
         <v>3</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -506,13 +509,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>